<commit_message>
Update test of chunck reader to test against real dates
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-batches-with-date.xlsx
+++ b/tests/Data/Disks/Local/import-batches-with-date.xlsx
@@ -21,15 +21,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -89,12 +91,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -115,10 +121,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -126,6 +132,11 @@
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
         <v>44896</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>44977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>